<commit_message>
Use open sans for article 7
</commit_message>
<xml_diff>
--- a/articles/article7/fonts_and_kerning.xlsx
+++ b/articles/article7/fonts_and_kerning.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\text_and_image_processing\article_generation\gitversion\articles\article7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamariorankins/repos/article_study/articles/article7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AAF0E7-E1CB-4071-A96F-8E3CA8E73CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578F2764-2F82-9646-8DB0-C0987D78F48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3240" windowWidth="24090" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="2720" windowWidth="24100" windowHeight="11660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
     <t>Kerning</t>
   </si>
   <si>
-    <t>Comic Sans</t>
+    <t>Open Sans</t>
   </si>
 </sst>
 </file>
@@ -397,12 +397,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:K5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>

</xml_diff>